<commit_message>
add listener, extendreport, CI/CD
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Berkas QA engineer\Bootcamp dibimbing.id\final Project Dibimbing\Final-project-automation-web\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A51E60-AC55-409C-90A9-5E780BF29FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5514F4DC-7C71-432C-A6FB-5BA71888647B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{5A5A1F02-D60F-45D4-9D26-0E53C2242333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="6" xr2:uid="{5A5A1F02-D60F-45D4-9D26-0E53C2242333}"/>
   </bookViews>
   <sheets>
     <sheet name="divisionData" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,11 @@
     <sheet name="addEmployee" sheetId="3" r:id="rId3"/>
     <sheet name="editEmployee" sheetId="4" r:id="rId4"/>
     <sheet name="addChapter" sheetId="7" r:id="rId5"/>
-    <sheet name="addTraining" sheetId="5" r:id="rId6"/>
-    <sheet name="editTraining" sheetId="6" r:id="rId7"/>
+    <sheet name="addContent" sheetId="8" r:id="rId6"/>
+    <sheet name="editContent" sheetId="10" r:id="rId7"/>
+    <sheet name="editChapter" sheetId="9" r:id="rId8"/>
+    <sheet name="addTraining" sheetId="5" r:id="rId9"/>
+    <sheet name="editTraining" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t xml:space="preserve">Division Name
 </t>
@@ -146,6 +149,30 @@
   </si>
   <si>
     <t>belajar sdlc dan stlc dasar</t>
+  </si>
+  <si>
+    <t>contentName</t>
+  </si>
+  <si>
+    <t>belajar sdlc</t>
+  </si>
+  <si>
+    <t>sldc</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>belajar sdlc dan stlc dasar dan menengah</t>
+  </si>
+  <si>
+    <t>Learn SDLC &amp; STLC tingkat lanjut</t>
+  </si>
+  <si>
+    <t>belajar sdlc untuk pemula</t>
+  </si>
+  <si>
+    <t>sldc dalam testing</t>
   </si>
 </sst>
 </file>
@@ -563,6 +590,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EA9D48-7011-44B9-A508-7541AF253141}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D319F093-F08A-4F4B-85F0-86F01EFC5A38}">
   <dimension ref="A1:B2"/>
@@ -796,13 +858,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD181E83-7BF9-4EAA-8AD4-E4E284C44DAC}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -827,6 +890,122 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C80B14-26EB-4D99-AF42-68F01AA5999A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F23CB20-3310-4499-8A19-656C20AABD8D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802048C9-FA8E-4A08-A2FA-87B86B75E329}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1942E1-D5F6-43B9-B053-E1A1963B1482}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -859,39 +1038,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EA9D48-7011-44B9-A508-7541AF253141}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
edit slack notifier error
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Berkas QA engineer\Bootcamp dibimbing.id\final Project Dibimbing\Final-project-automation-web\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E52ED1-0AC5-4DE6-9B0C-C8CFB3BC34F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFDCB49-36FB-465A-A786-598CF36608CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{5A5A1F02-D60F-45D4-9D26-0E53C2242333}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5A5A1F02-D60F-45D4-9D26-0E53C2242333}"/>
   </bookViews>
   <sheets>
     <sheet name="divisionData" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="49">
   <si>
     <t xml:space="preserve">Division Name
 </t>
@@ -62,12 +62,6 @@
  performance.</t>
   </si>
   <si>
-    <t>division business Team</t>
-  </si>
-  <si>
-    <t>business</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -201,6 +195,9 @@
   </si>
   <si>
     <t>correctAnswer</t>
+  </si>
+  <si>
+    <t>division business Team test edit data</t>
   </si>
 </sst>
 </file>
@@ -644,42 +641,42 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="F1" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="F2" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,18 +708,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -734,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D319F093-F08A-4F4B-85F0-86F01EFC5A38}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,12 +749,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -785,54 +782,54 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>85666111222111</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
         <v>37289</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <v>1928753418263410</v>
@@ -843,31 +840,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -899,51 +896,51 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2">
         <v>85667866761</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
         <v>37289</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H2">
         <v>192876767534182</v>
@@ -973,18 +970,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1008,21 +1005,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -1048,21 +1045,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2">
         <v>50</v>
@@ -1077,7 +1074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802048C9-FA8E-4A08-A2FA-87B86B75E329}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1089,18 +1086,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1124,18 +1121,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>